<commit_message>
Finish 1NF in Exercise 2 lab 04
</commit_message>
<xml_diff>
--- a/Homework 04/Ans_Hw_04_Ex_2.xlsx
+++ b/Homework 04/Ans_Hw_04_Ex_2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>UNF</t>
   </si>
@@ -62,9 +62,6 @@
     <t>LaborTax</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>MaterialDetail</t>
   </si>
   <si>
@@ -81,6 +78,24 @@
   </si>
   <si>
     <t>TotalAmount</t>
+  </si>
+  <si>
+    <t>CusID</t>
+  </si>
+  <si>
+    <t>MaterialID</t>
+  </si>
+  <si>
+    <t>TaxAmount</t>
+  </si>
+  <si>
+    <t>LaborNo</t>
+  </si>
+  <si>
+    <t>TotalLaborAmount</t>
+  </si>
+  <si>
+    <t>TotalMatAmount</t>
   </si>
 </sst>
 </file>
@@ -96,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +121,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -146,11 +167,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -167,6 +193,548 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="523875" y="2038350"/>
+          <a:ext cx="10325100" cy="2628900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200"/>
+            <a:t>1NF</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t> :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>({InvoiceID,LaborNo,MaterialNo}</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> PK</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>, Date,CusName,CusAddr,CusPhone,CusEmail,LaborNo,LaborDetail,LaborRate,LaborHours,LaborAmount</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>LaborTax,TaxAmount,LaborAmount,TotalLaborAmount,MaterialID,MaterialName,MaterialDetail,MaterialPrice,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MaterialAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MaterialTax</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TaxAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TotalMatAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TotalAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>2NF :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>Invoice({InvoiceID} PK, CusID,LaborNo,MaterialNo,Date,TotalAmount)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>Labor({LaborID} PK, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LaborDetail</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LaborRate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LaborHours</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LaborAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LaborTax</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TaxAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TotalLaborAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>Material({MaterialID} PK, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MaterialPrice</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MaterialQuantities</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MaterialAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>MaterialTax</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TaxAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TotalMatAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TotalAmount</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>InvoiceLaborDetail({InvoiceID} PK,LaborNo)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" baseline="0"/>
+            <a:t>InvoiceMaterialDetail({InvoiceID} PK, MaterialID)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7:V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,18 +1018,20 @@
     <col min="8" max="8" width="17.140625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="18.42578125" customWidth="1"/>
+    <col min="11" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="19" width="19.5703125" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="18.42578125" customWidth="1"/>
+    <col min="22" max="22" width="17.85546875" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -483,8 +1053,10 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -519,34 +1091,262 @@
         <v>11</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S2" s="1" t="s">
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>